<commit_message>
refactor: Update visualization script and improve code structure
</commit_message>
<xml_diff>
--- a/grid_analysis_report.xlsx
+++ b/grid_analysis_report.xlsx
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>47.62</v>
+        <v>23.9</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -890,19 +890,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>47.62</v>
+        <v>23.9</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Sargassum vulgare</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>0.253</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Latest update to test the frame seg on one-zero shot
</commit_message>
<xml_diff>
--- a/grid_analysis_report.xlsx
+++ b/grid_analysis_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Grid Analysis" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Coverage Analysis" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,37 +446,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Grid Cell Area (cm²)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Total Coverage (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cystoseira sl Coverage (%)</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Posidonia oceanica Coverage (%)</t>
+          <t>blueberry Coverage (%)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Sargassum vulgare Coverage (%)</t>
+          <t>blueberry Area (cm²)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>lingonberry Coverage (%)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>lingonberry Area (cm²)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>crowberry Coverage (%)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>crowberry Area (cm²)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>frame Coverage (%)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>frame Area (cm²)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>wood / stick Coverage (%)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>wood / stick Area (cm²)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Total Detections</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Det_1_Class</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Det_1_Confidence</t>
         </is>
       </c>
     </row>
@@ -488,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>76.34999999999999</v>
+        <v>156.25</v>
       </c>
       <c r="D2" t="n">
-        <v>76.34999999999999</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -500,15 +530,31 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Cystoseira sl</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9717</v>
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -519,22 +565,44 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>50.11</v>
+        <v>156.25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.87</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>49.24</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -544,22 +612,44 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>89.5</v>
+        <v>156.25</v>
       </c>
       <c r="D4" t="n">
-        <v>15.53</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>73.97</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -569,10 +659,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>156.25</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -583,8 +673,30 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -594,22 +706,44 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>90.83</v>
+        <v>156.25</v>
       </c>
       <c r="D6" t="n">
-        <v>63.07</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>27.77</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -619,22 +753,44 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>98.98</v>
+        <v>156.25</v>
       </c>
       <c r="D7" t="n">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>93.38</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -644,22 +800,44 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>93.08</v>
+        <v>156.25</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>92.88</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -669,27 +847,43 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>93.43000000000001</v>
+        <v>156.25</v>
       </c>
       <c r="D9" t="n">
-        <v>50.4</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>43.02</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Cystoseira sl</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9695</v>
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -700,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>156.25</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -709,13 +903,35 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -725,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>156.25</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -734,18 +950,34 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Sargassum vulgare</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9752</v>
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -756,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>156.25</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -765,13 +997,35 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -781,22 +1035,44 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>81.52</v>
+        <v>156.25</v>
       </c>
       <c r="D13" t="n">
-        <v>11.44</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>70.08</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -806,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>35.42</v>
+        <v>156.25</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -815,13 +1091,35 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>35.42</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -831,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>55.37</v>
+        <v>156.25</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -840,13 +1138,35 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>55.37</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -856,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>94.03</v>
+        <v>156.25</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -865,13 +1185,35 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>94.03</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -881,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>23.9</v>
+        <v>156.25</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -890,13 +1232,35 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>23.9</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update image path in photo_analysis.py and refresh analysis files
</commit_message>
<xml_diff>
--- a/grid_analysis_report.xlsx
+++ b/grid_analysis_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Coverage Analysis" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Grid Analysis" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,67 +446,37 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Grid Cell Area (cm²)</t>
+          <t>Total Coverage (%)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Total Coverage (%)</t>
+          <t>Cystoseira sl Coverage (%)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>blueberry Coverage (%)</t>
+          <t>Posidonia oceanica Coverage (%)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>blueberry Area (cm²)</t>
+          <t>Sargassum vulgare Coverage (%)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>lingonberry Coverage (%)</t>
+          <t>Total Detections</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>lingonberry Area (cm²)</t>
+          <t>Det_1_Class</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>crowberry Coverage (%)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>crowberry Area (cm²)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>frame Coverage (%)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>frame Area (cm²)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>wood / stick Coverage (%)</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>wood / stick Area (cm²)</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Total Detections</t>
+          <t>Det_1_Confidence</t>
         </is>
       </c>
     </row>
@@ -518,10 +488,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>156.25</v>
+        <v>76.34999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>76.34999999999999</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -530,31 +500,15 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Cystoseira sl</t>
+        </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
+        <v>0.9717</v>
       </c>
     </row>
     <row r="3">
@@ -565,44 +519,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>156.25</v>
+        <v>50.11</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>49.24</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -612,44 +544,22 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>156.25</v>
+        <v>89.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>15.53</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>73.97</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -659,10 +569,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>156.25</v>
+        <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -673,30 +583,8 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -706,44 +594,22 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>156.25</v>
+        <v>90.83</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>63.07</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>27.77</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -753,44 +619,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>156.25</v>
+        <v>98.98</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>93.38</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -800,44 +644,22 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>156.25</v>
+        <v>93.08</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>92.88</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -847,43 +669,27 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>156.25</v>
+        <v>93.43000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>50.4</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>43.02</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Cystoseira sl</t>
+        </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
+        <v>0.9695</v>
       </c>
     </row>
     <row r="10">
@@ -894,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>156.25</v>
+        <v>100</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -903,35 +709,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -941,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>156.25</v>
+        <v>100</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -950,34 +734,18 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Sargassum vulgare</t>
+        </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
+        <v>0.9752</v>
       </c>
     </row>
     <row r="12">
@@ -988,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>156.25</v>
+        <v>100</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -997,35 +765,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1035,44 +781,22 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>156.25</v>
+        <v>81.52</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>11.44</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>70.08</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1082,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>156.25</v>
+        <v>35.42</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1091,35 +815,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>35.42</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1129,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>156.25</v>
+        <v>55.37</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -1138,35 +840,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>55.37</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1176,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>156.25</v>
+        <v>94.03</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -1185,35 +865,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>94.03</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1223,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>156.25</v>
+        <v>23.9</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1232,35 +890,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>23.9</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>